<commit_message>
subido antes de la revision con el ecn
</commit_message>
<xml_diff>
--- a/Paises.xlsx
+++ b/Paises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive .Edu\Resilencia_AL_COVID19\Resilencia_R-Studio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive .Edu\Resilencia_AL_COVID19\GitHub\mrclofrndz16.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0252B80-BF39-49CF-A427-34FB50C25F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529E57A-7863-4437-BF74-C53E94C3D99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{598346EE-8392-4228-BAAB-26705E51897A}"/>
+    <workbookView xWindow="7590" yWindow="2655" windowWidth="7500" windowHeight="6000" xr2:uid="{598346EE-8392-4228-BAAB-26705E51897A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="50">
   <si>
     <t>Antigua and Barbuda</t>
   </si>
@@ -341,9 +341,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Countries</t>
-  </si>
-  <si>
     <t>WEO</t>
   </si>
   <si>
@@ -375,13 +372,19 @@
   </si>
   <si>
     <t>Paises Finales</t>
+  </si>
+  <si>
+    <t>Countries all América</t>
+  </si>
+  <si>
+    <t>America Latina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,14 +393,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -463,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -471,13 +466,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -884,67 +876,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBDB4DA-06BE-40F9-B76F-42B4E7B9F29E}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1"/>
+    <col min="1" max="1" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="1"/>
-    <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="1"/>
-    <col min="6" max="6" width="3" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="1"/>
-    <col min="10" max="10" width="3" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.42578125" style="1"/>
+    <col min="10" max="10" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1"/>
+    <col min="12" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,8 +962,8 @@
         <f t="shared" ref="F2:F37" si="1">+IF($A2=E2,"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>45</v>
+      <c r="G2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="str">
         <f t="shared" ref="H2:H37" si="2">+IF($A2=G2,"SI","NO")</f>
@@ -983,8 +980,11 @@
         <f>+IF(H2="NO","NO HAY EN ILE",A2)</f>
         <v>NO HAY EN ILE</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1023,8 +1023,11 @@
         <f t="shared" ref="K3:K37" si="4">+IF(H3="NO","NO HAY EN ILE",A3)</f>
         <v>Argentina</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1063,8 +1066,11 @@
         <f t="shared" si="4"/>
         <v>Barbados</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1103,8 +1109,11 @@
         <f t="shared" si="4"/>
         <v>Belize</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1132,7 +1141,7 @@
         <f t="shared" si="2"/>
         <v>SI</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="1" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
@@ -1141,8 +1150,11 @@
         <f t="shared" si="4"/>
         <v>Bolivia</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1181,8 +1193,11 @@
         <f t="shared" si="4"/>
         <v>Brazil</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1221,8 +1236,11 @@
         <f t="shared" si="4"/>
         <v>Canada</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1268,7 @@
         <f t="shared" si="2"/>
         <v>SI</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -1261,8 +1279,11 @@
         <f t="shared" si="4"/>
         <v>Chile</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1301,8 +1322,11 @@
         <f t="shared" si="4"/>
         <v>Colombia</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1341,15 +1365,18 @@
         <f t="shared" si="4"/>
         <v>Costa Rica</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
@@ -1361,7 +1388,7 @@
         <f t="shared" si="1"/>
         <v>SI</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -1377,8 +1404,11 @@
         <f t="shared" si="4"/>
         <v>NO HAY EN ILE</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1429,7 @@
         <f t="shared" si="1"/>
         <v>SI</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -1415,8 +1445,11 @@
         <f t="shared" si="4"/>
         <v>NO HAY EN ILE</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1455,8 +1488,11 @@
         <f t="shared" si="4"/>
         <v>Dominican Republic</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1495,8 +1531,11 @@
         <f t="shared" si="4"/>
         <v>Ecuador</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1535,25 +1574,28 @@
         <f t="shared" si="4"/>
         <v>El Salvador</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="1" t="str">
         <f t="shared" si="5"/>
         <v>NO</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>NO</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -1566,8 +1608,11 @@
         <f t="shared" si="4"/>
         <v>NO HAY EN ILE</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1633,7 @@
         <f t="shared" si="1"/>
         <v>SI</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -1604,8 +1649,11 @@
         <f t="shared" si="4"/>
         <v>NO HAY EN ILE</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1644,8 +1692,11 @@
         <f t="shared" si="4"/>
         <v>Guatemala</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1684,8 +1735,11 @@
         <f t="shared" si="4"/>
         <v>Guyana</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1724,8 +1778,11 @@
         <f t="shared" si="4"/>
         <v>Haiti</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1765,7 +1822,7 @@
         <v>Honduras</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1862,7 @@
         <v>Jamaica</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -1845,7 +1902,7 @@
         <v>Mexico</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1885,7 +1942,7 @@
         <v>Nicaragua</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1925,7 +1982,7 @@
         <v>Panama</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1965,7 +2022,7 @@
         <v>Paraguay</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2005,24 +2062,24 @@
         <v>Peru</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1" t="str">
         <f t="shared" si="5"/>
         <v>NO</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>NO</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -2039,24 +2096,24 @@
         <v>NO HAY EN ILE</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="1" t="str">
         <f t="shared" si="5"/>
         <v>NO</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="1" t="str">
         <f t="shared" si="1"/>
         <v>NO</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -2073,24 +2130,24 @@
         <v>NO HAY EN ILE</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="1" t="str">
         <f t="shared" si="5"/>
         <v>NO</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="1" t="str">
         <f t="shared" si="1"/>
         <v>NO</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
@@ -2107,7 +2164,7 @@
         <v>NO HAY EN ILE</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2147,29 +2204,29 @@
         <v>Suriname</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="1" t="str">
         <f t="shared" si="5"/>
         <v>NO</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="1" t="str">
         <f t="shared" si="1"/>
         <v>NO</v>
       </c>
-      <c r="G33" s="8"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
       </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="1" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
@@ -2327,7 +2384,7 @@
         <f t="shared" si="2"/>
         <v>SI</v>
       </c>
-      <c r="I37" s="6"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="1" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
@@ -2338,53 +2395,21 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K37" xr:uid="{EAA24AFF-158C-4CF1-95F2-39CE24CD1E17}">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="Argentina"/>
-        <filter val="Barbados"/>
-        <filter val="Belize"/>
-        <filter val="Bolivia"/>
-        <filter val="Brazil"/>
-        <filter val="Canada"/>
-        <filter val="Chile"/>
-        <filter val="Colombia"/>
-        <filter val="Costa Rica"/>
-        <filter val="Dominican Republic"/>
-        <filter val="Ecuador"/>
-        <filter val="El Salvador"/>
-        <filter val="Guatemala"/>
-        <filter val="Guyana"/>
-        <filter val="Haiti"/>
-        <filter val="Honduras"/>
-        <filter val="Jamaica"/>
-        <filter val="Mexico"/>
-        <filter val="Nicaragua"/>
-        <filter val="Panama"/>
-        <filter val="Paraguay"/>
-        <filter val="Peru"/>
-        <filter val="Suriname"/>
-        <filter val="Trinidad and Tobago"/>
-        <filter val="United States"/>
-        <filter val="Uruguay"/>
-        <filter val="Venezuela"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J37">
-    <sortCondition ref="A1"/>
+  <autoFilter ref="A1:K37" xr:uid="{EAA24AFF-158C-4CF1-95F2-39CE24CD1E17}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:L22">
+    <sortCondition ref="L2"/>
   </sortState>
   <conditionalFormatting sqref="D1">
     <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">

</xml_diff>